<commit_message>
Update TO DO LIST Dec 23 - Mar 24.xlsx
Updated line items
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/TO DO LIST Dec 23 - Mar 24.xlsx
+++ b/Offline/BusinessManagement/Marketing/TO DO LIST Dec 23 - Mar 24.xlsx
@@ -44,15 +44,9 @@
     <t>Bappadittya Debsingha</t>
   </si>
   <si>
-    <t>Python, Hardware Optimized Coding, Data Analysis, Data Visualization, AI Theory &amp; Ethics, Generative AI, Prompt Engineering</t>
-  </si>
-  <si>
     <t>Sayan Basak</t>
   </si>
   <si>
-    <t>Mathematics &amp; Statistics, Data Science Practical, Neural Networks, Optimization and Project organisation, MLOPS, AWS Sagemaker, CV/CNN, RNN, TF, Keras, Pytorch, DSP</t>
-  </si>
-  <si>
     <t>Anirban Chakraborty</t>
   </si>
   <si>
@@ -60,6 +54,12 @@
   </si>
   <si>
     <t>Rahul Dutta &amp; Srinjina Mukherjee</t>
+  </si>
+  <si>
+    <t>Python, Hardware Optimized Coding, Data Analysis, Data Visualization, AI Theory &amp; Ethics, Generative AI, Prompt Engineering, Additive Color Mixing (RGB), Number System, Logic Gates</t>
+  </si>
+  <si>
+    <t>Mathematics &amp; Statistics, Data Science Practical, Neural Networks, Optimization and Project organisation, MLOPS, AWS Sagemaker, CV/CNN, RNN, TF, Keras, Pytorch, DSP, Additive Color Mixing (RGB), Number System, Logic Gates</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -123,11 +123,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="3"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top style="thick">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3"/>
+      </left>
+      <right style="thick">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -139,6 +176,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -421,15 +476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I1:J8"/>
+  <dimension ref="I1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="38" customWidth="1"/>
+    <col min="9" max="9" width="54" customWidth="1"/>
     <col min="10" max="10" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -442,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="9:10" ht="263.39999999999998" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="9:10" ht="100.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -450,7 +505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="9:10" ht="84" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="9:10" ht="100.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
@@ -458,32 +513,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="9:10" ht="249.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="9:10" ht="100.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="4" t="s">
+    </row>
+    <row r="6" spans="9:10" ht="100.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="9:10" ht="332.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I6" s="2" t="s">
+    <row r="7" spans="9:10" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="9:10" ht="139.19999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="9:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="9:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="9:10" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="9:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>